<commit_message>
Changed string datetimes to type DateTime?
</commit_message>
<xml_diff>
--- a/src/WMOSS-EXCELDB-SAMPLE.xlsx
+++ b/src/WMOSS-EXCELDB-SAMPLE.xlsx
@@ -16,11 +16,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+  <si>
+    <t>FULLNAME</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>PASSWORD_ENCRYPTED</t>
+  </si>
+  <si>
+    <t>ROLE</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
   <si>
     <t>TITLE</t>
   </si>
   <si>
+    <t>CAPACITY</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
     <t>RELEASE_DATE</t>
   </si>
   <si>
@@ -42,25 +63,16 @@
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t>CAPACITY</t>
-  </si>
-  <si>
-    <t>ADDRESS</t>
-  </si>
-  <si>
-    <t>FULLNAME</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>PASSWORD_ENCRYPTED</t>
-  </si>
-  <si>
-    <t>ROLE</t>
+    <t>Mission: Impossible - Fallout</t>
+  </si>
+  <si>
+    <t>Action, Adventure, Thriller</t>
+  </si>
+  <si>
+    <t>PG-13</t>
+  </si>
+  <si>
+    <t>Ethan Hunt and his IMF team, along with some familiar allies, race against time after a mission gone wrong.</t>
   </si>
   <si>
     <t>MOVIE_ID</t>
@@ -106,6 +118,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy hh:mm:ss"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -128,11 +143,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -180,16 +198,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -224,33 +242,56 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="I1" s="1"/>
     </row>
-  </sheetData>
-  <dataValidations>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2">
+        <v>43308.0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1">
+        <v>140.0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid date" sqref="B2:B952">
+      <formula1>OR(NOT(ISERROR(DATEVALUE(B2))), AND(ISNUMBER(B2), LEFT(CELL("format", B2))="D"))</formula1>
+    </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" prompt="Enter a number between 1 and 9999" sqref="G2:G952">
       <formula1>1.0</formula1>
       <formula2>9999.0</formula2>
@@ -280,13 +321,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -317,22 +358,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -343,6 +384,9 @@
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than or equal to 2" sqref="A2:B940 E2:E940">
       <formula1>2.0</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid date and time" sqref="C2:C940 F2:F940">
+      <formula1>OR(NOT(ISERROR(DATEVALUE(C2))), AND(ISNUMBER(C2), LEFT(CELL("format", C2))="D"))</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
@@ -363,31 +407,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than or equal to 0.00" sqref="D2:D970">
       <formula1>0.0</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid date and time" sqref="G2:G970">
+      <formula1>OR(NOT(ISERROR(DATEVALUE(G2))), AND(ISNUMBER(G2), LEFT(CELL("format", G2))="D"))</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" prompt="Enter a valid email" sqref="C2:C970">
       <formula1>IFERROR(ISEMAIL(C2), true)</formula1>
@@ -411,13 +458,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="D1" s="1"/>
     </row>

</xml_diff>